<commit_message>
Spreadsheet adapted to 6V supercap
</commit_message>
<xml_diff>
--- a/bq25505(70_Design_Help_V1_3.xlsx
+++ b/bq25505(70_Design_Help_V1_3.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nagercoin/workspace/kicad/BQ25570EVM/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577E1967-602F-424E-BE35-08240163D48E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="270" windowWidth="17790" windowHeight="7815"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bq25505(70" sheetId="1" r:id="rId1"/>
@@ -18,7 +24,7 @@
     <definedName name="VOUT">'bq25505(70'!#REF!</definedName>
     <definedName name="VPGOOD">'bq25505(70'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -521,7 +527,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -1258,6 +1264,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1282,9 +1291,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1294,6 +1300,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1316,7 +1325,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1363,7 +1378,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1410,7 +1431,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="Straight Arrow Connector 9"/>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1457,7 +1484,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="Straight Arrow Connector 11"/>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1504,7 +1537,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Straight Arrow Connector 14"/>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1551,7 +1590,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="Straight Arrow Connector 15"/>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1598,7 +1643,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="Straight Arrow Connector 17"/>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1645,7 +1696,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="20" name="Straight Arrow Connector 19"/>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1692,7 +1749,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="Straight Arrow Connector 16"/>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1739,7 +1802,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="24" name="Straight Arrow Connector 23"/>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1778,13 +1847,13 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>114300</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
+          <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>22</xdr:col>
-          <xdr:colOff>104775</xdr:colOff>
+          <xdr:colOff>101600</xdr:colOff>
           <xdr:row>65</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>165100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1793,11 +1862,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1805,6 +1877,17 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1858,7 +1941,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1891,9 +1974,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1926,6 +2026,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2101,38 +2218,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F18" sqref="F18"/>
+      <selection pane="topRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="11" width="8.7109375" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" customWidth="1"/>
-    <col min="13" max="13" width="2.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" customWidth="1"/>
-    <col min="16" max="17" width="8.7109375" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" customWidth="1"/>
-    <col min="19" max="19" width="2.7109375" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" customWidth="1"/>
-    <col min="21" max="21" width="6.7109375" customWidth="1"/>
-    <col min="22" max="24" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" customWidth="1"/>
+    <col min="10" max="11" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" customWidth="1"/>
+    <col min="13" max="13" width="2.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" customWidth="1"/>
+    <col min="16" max="17" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="6.6640625" customWidth="1"/>
+    <col min="19" max="19" width="2.6640625" customWidth="1"/>
+    <col min="20" max="20" width="12.6640625" customWidth="1"/>
+    <col min="21" max="21" width="6.6640625" customWidth="1"/>
+    <col min="22" max="24" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
@@ -2146,12 +2263,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="69"/>
       <c r="B3" s="36" t="s">
         <v>54</v>
@@ -2182,7 +2299,7 @@
       <c r="W3" s="37"/>
       <c r="X3" s="38"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="69"/>
       <c r="B4" s="50" t="s">
         <v>23</v>
@@ -2214,7 +2331,7 @@
       <c r="W4" s="3"/>
       <c r="X4" s="40"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="69"/>
       <c r="B5" s="42" t="s">
         <v>55</v>
@@ -2242,37 +2359,37 @@
       <c r="W5" s="71"/>
       <c r="X5" s="74"/>
     </row>
-    <row r="6" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="95" t="s">
+    <row r="6" spans="1:24" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="97"/>
-      <c r="H6" s="98" t="s">
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="100"/>
+      <c r="H6" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="99"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="100"/>
-      <c r="N6" s="98" t="s">
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="103"/>
+      <c r="N6" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="O6" s="99"/>
-      <c r="P6" s="99"/>
-      <c r="Q6" s="99"/>
-      <c r="R6" s="100"/>
-      <c r="T6" s="98" t="s">
+      <c r="O6" s="102"/>
+      <c r="P6" s="102"/>
+      <c r="Q6" s="102"/>
+      <c r="R6" s="103"/>
+      <c r="T6" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="99"/>
-      <c r="V6" s="99"/>
-      <c r="W6" s="99"/>
-      <c r="X6" s="100"/>
-    </row>
-    <row r="7" spans="1:24" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="U6" s="102"/>
+      <c r="V6" s="102"/>
+      <c r="W6" s="102"/>
+      <c r="X6" s="103"/>
+    </row>
+    <row r="7" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="85" t="s">
         <v>27</v>
       </c>
@@ -2309,7 +2426,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="17"/>
     </row>
-    <row r="8" spans="1:24" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="34" t="s">
         <v>27</v>
       </c>
@@ -2328,7 +2445,7 @@
         <v>8</v>
       </c>
       <c r="I8" s="13">
-        <v>2.8</v>
+        <v>1.3</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>1</v>
@@ -2362,7 +2479,7 @@
       </c>
       <c r="X8" s="17"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="34" t="s">
         <v>27</v>
       </c>
@@ -2370,7 +2487,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="13">
-        <v>4.2</v>
+        <v>5.5</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>1</v>
@@ -2381,7 +2498,7 @@
         <v>20</v>
       </c>
       <c r="I9" s="13">
-        <v>3.1</v>
+        <v>1.5</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>1</v>
@@ -2394,7 +2511,7 @@
         <v>44</v>
       </c>
       <c r="O9" s="13">
-        <v>1.3</v>
+        <v>3.5</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>1</v>
@@ -2415,7 +2532,7 @@
       </c>
       <c r="X9" s="17"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B10" s="19"/>
       <c r="C10" s="30"/>
       <c r="D10" s="18"/>
@@ -2437,7 +2554,7 @@
       <c r="W10" s="18"/>
       <c r="X10" s="17"/>
     </row>
-    <row r="11" spans="1:24" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="19"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
@@ -2445,10 +2562,10 @@
       <c r="F11" s="17"/>
       <c r="H11" s="19"/>
       <c r="I11" s="18"/>
-      <c r="J11" s="101" t="s">
+      <c r="J11" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="K11" s="102"/>
+      <c r="K11" s="105"/>
       <c r="L11" s="17"/>
       <c r="N11" s="19"/>
       <c r="O11" s="18"/>
@@ -2457,19 +2574,19 @@
       <c r="R11" s="17"/>
       <c r="T11" s="19"/>
       <c r="U11" s="18"/>
-      <c r="V11" s="101" t="s">
+      <c r="V11" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="W11" s="102"/>
+      <c r="W11" s="105"/>
       <c r="X11" s="17"/>
     </row>
-    <row r="12" spans="1:24" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="19"/>
       <c r="C12" s="18"/>
-      <c r="D12" s="101" t="s">
+      <c r="D12" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="102"/>
+      <c r="E12" s="105"/>
       <c r="F12" s="17"/>
       <c r="H12" s="19"/>
       <c r="I12" s="51" t="s">
@@ -2484,10 +2601,10 @@
       <c r="L12" s="17"/>
       <c r="N12" s="19"/>
       <c r="O12" s="18"/>
-      <c r="P12" s="101" t="s">
+      <c r="P12" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="Q12" s="102"/>
+      <c r="Q12" s="105"/>
       <c r="R12" s="17"/>
       <c r="T12" s="19"/>
       <c r="U12" s="51" t="s">
@@ -2501,7 +2618,7 @@
       </c>
       <c r="X12" s="17"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="34" t="s">
         <v>25</v>
       </c>
@@ -2521,15 +2638,15 @@
       </c>
       <c r="I13" s="31">
         <f>C1/I9*I7</f>
-        <v>5.0741935483870968</v>
+        <v>10.486666666666666</v>
       </c>
       <c r="J13" s="52">
         <f>IF(I13&gt;1,VLOOKUP(I13*10,$AA$27:$AA$133,1)/10,IF(I13&gt;0.099,VLOOKUP(I13*100,$AB$27:$AB$133,1)/100,VLOOKUP(I13*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>4.99</v>
+        <v>10</v>
       </c>
       <c r="K13" s="52">
         <f ca="1">IF(I13&gt;1,OFFSET($AA$27,MATCH(I13*10,$AA$27:$AA$133,1),0)/10,IF(I13&gt;0.099, OFFSET($AB$27,MATCH(I13*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(I13*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>5.1100000000000003</v>
+        <v>0</v>
       </c>
       <c r="L13" s="54" t="s">
         <v>59</v>
@@ -2564,7 +2681,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="34" t="s">
         <v>25</v>
       </c>
@@ -2573,15 +2690,15 @@
       </c>
       <c r="C14" s="31">
         <f>C8*$C$1/C9*3/2</f>
-        <v>5.6178571428571429</v>
+        <v>4.29</v>
       </c>
       <c r="D14" s="52">
         <f>IF(C14&gt;1,VLOOKUP(C14*10,$AA$27:$AA$133,1)/10,IF(C14&gt;0.099,VLOOKUP(C14*100,$AB$27:$AB$133,1)/100,VLOOKUP(C14*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>5.49</v>
+        <v>4.2200000000000006</v>
       </c>
       <c r="E14" s="52">
         <f ca="1">IF(C14&gt;1,OFFSET($AA$27,MATCH(C14*10,$AA$27:$AA$133,1),0)/10,IF(C14&gt;0.099, OFFSET($AB$27,MATCH(C14*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(C14*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>5.62</v>
+        <v>4.32</v>
       </c>
       <c r="F14" s="54" t="s">
         <v>59</v>
@@ -2591,15 +2708,15 @@
       </c>
       <c r="I14" s="31">
         <f>(I8/C1-1)*I13</f>
-        <v>6.6677419354838703</v>
+        <v>0.77999999999999969</v>
       </c>
       <c r="J14" s="52">
         <f>IF(I14&gt;1,VLOOKUP(I14*10,$AA$27:$AA$133,1)/10,IF(I14&gt;0.099,VLOOKUP(I14*100,$AB$27:$AB$133,1)/100,VLOOKUP(I14*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>6.65</v>
+        <v>0.76800000000000002</v>
       </c>
       <c r="K14" s="52">
         <f ca="1">IF(I14&gt;1,OFFSET($AA$27,MATCH(I14*10,$AA$27:$AA$133,1),0)/10,IF(I14&gt;0.099, OFFSET($AB$27,MATCH(I14*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(I14*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>6.81</v>
+        <v>0.78700000000000003</v>
       </c>
       <c r="L14" s="54" t="s">
         <v>59</v>
@@ -2609,15 +2726,15 @@
       </c>
       <c r="O14" s="31">
         <f>IF(O8*$C$1/O9&lt;=10, O8*$C$1/O9, O8*$C$1/O9-10)</f>
-        <v>2.0999999999999996</v>
+        <v>4.4942857142857147</v>
       </c>
       <c r="P14" s="52">
         <f>IF(O14&gt;1,VLOOKUP(O14*10,$AA$26:$AA$132,1)/10,IF(O14&gt;0.099,VLOOKUP(O14*100,$AB$26:$AB$132,1)/100,VLOOKUP(O14*1000,$AB$26:$AB$132,1)/1000))</f>
-        <v>2.0499999999999998</v>
+        <v>4.42</v>
       </c>
       <c r="Q14" s="52">
         <f ca="1">IF(O14&gt;1,OFFSET($AA$26,MATCH(O14*10,$AA$26:$AA$132,1),0)/10,IF(O14&gt;0.099, OFFSET($AB$26,MATCH(O14*100,$AB$26:$AB$132,1),0)/100,OFFSET($AB$26,MATCH(O14*1000,$AB$26:$AB$132,1),0)/1000))</f>
-        <v>2.1</v>
+        <v>4.5299999999999994</v>
       </c>
       <c r="R14" s="54" t="s">
         <v>59</v>
@@ -2641,7 +2758,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="34" t="s">
         <v>25</v>
       </c>
@@ -2650,15 +2767,15 @@
       </c>
       <c r="C15" s="31">
         <f>C8-C14</f>
-        <v>7.3821428571428571</v>
+        <v>8.7100000000000009</v>
       </c>
       <c r="D15" s="52">
         <f>IF(C15&gt;1,VLOOKUP(C15*10,$AA$27:$AA$133,1)/10,IF(C15&gt;0.099,VLOOKUP(C15*100,$AB$27:$AB$133,1)/100,VLOOKUP(C15*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>7.32</v>
+        <v>8.66</v>
       </c>
       <c r="E15" s="52">
         <f ca="1">IF(C15&gt;1,OFFSET($AA$27,MATCH(C15*10,$AA$27:$AA$133,1),0)/10,IF(C15&gt;0.099, OFFSET($AB$27,MATCH(C15*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(C15*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>7.5</v>
+        <v>8.870000000000001</v>
       </c>
       <c r="F15" s="54" t="s">
         <v>59</v>
@@ -2668,15 +2785,15 @@
       </c>
       <c r="I15" s="31">
         <f>I7-I13-I14</f>
-        <v>1.2580645161290329</v>
+        <v>1.7333333333333338</v>
       </c>
       <c r="J15" s="52">
         <f>IF(I15&gt;1,VLOOKUP(I15*10,$AA$27:$AA$133,1)/10,IF(I15&gt;0.099,VLOOKUP(I15*100,$AB$27:$AB$133,1)/100,VLOOKUP(I15*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>1.1300000000000001</v>
+        <v>1.69</v>
       </c>
       <c r="K15" s="52">
         <f ca="1">IF(I15&gt;1,OFFSET($AA$27,MATCH(I15*10,$AA$27:$AA$133,1),0)/10,IF(I15&gt;0.099, OFFSET($AB$27,MATCH(I15*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(I15*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>1.27</v>
+        <v>1.7399999999999998</v>
       </c>
       <c r="L15" s="54" t="s">
         <v>59</v>
@@ -2686,15 +2803,15 @@
       </c>
       <c r="O15" s="91">
         <f>IF(O8*$C$1/O9&lt;=10,0,10)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P15" s="57">
         <f>IF(O8*$C$1/O9&lt;=10,0,10)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="57">
         <f>IF(O8*$C$1/O9&lt;=10,0,10)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="R15" s="54" t="s">
         <v>59</v>
@@ -2718,7 +2835,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="34" t="s">
         <v>25</v>
       </c>
@@ -2728,11 +2845,11 @@
       <c r="C16" s="32"/>
       <c r="D16" s="53">
         <f>C1*(1+D15/D14)*3/2</f>
-        <v>4.2349999999999994</v>
+        <v>5.5396208530805673</v>
       </c>
       <c r="E16" s="53">
         <f ca="1">C1*(1+E15/E14)*3/2</f>
-        <v>4.2371530249110325</v>
+        <v>5.5416319444444451</v>
       </c>
       <c r="F16" s="83" t="s">
         <v>1</v>
@@ -2743,11 +2860,11 @@
       <c r="I16" s="18"/>
       <c r="J16" s="53">
         <f>C1*(1+J14/J13)</f>
-        <v>2.8225250501002006</v>
-      </c>
-      <c r="K16" s="53">
+        <v>1.3029279999999999</v>
+      </c>
+      <c r="K16" s="53" t="e">
         <f ca="1">C1*(1+K14/K13)</f>
-        <v>2.8225440313111543</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L16" s="83" t="s">
         <v>1</v>
@@ -2757,15 +2874,15 @@
       </c>
       <c r="O16" s="31">
         <f>IF(O8*$C$1/O9&lt;=10, O8-O14, O8-O14-10)</f>
-        <v>0.90000000000000036</v>
+        <v>8.5057142857142853</v>
       </c>
       <c r="P16" s="52">
         <f>IF(O16&gt;1,VLOOKUP(O16*10,$AA$26:$AA$132,1)/10,IF(O16&gt;0.099,VLOOKUP(O16*100,$AB$26:$AB$132,1)/100,VLOOKUP(O16*1000,$AB$26:$AB$132,1)/1000))</f>
-        <v>0.88700000000000001</v>
+        <v>8.4499999999999993</v>
       </c>
       <c r="Q16" s="52">
         <f ca="1">IF(O16&gt;1,OFFSET($AA$26,MATCH(O16*10,$AA$26:$AA$132,1),0)/10,IF(O16&gt;0.099, OFFSET($AB$26,MATCH(O16*100,$AB$26:$AB$132,1),0)/100,OFFSET($AB$26,MATCH(O16*1000,$AB$26:$AB$132,1),0)/1000))</f>
-        <v>0.90900000000000003</v>
+        <v>8.66</v>
       </c>
       <c r="R16" s="54" t="s">
         <v>59</v>
@@ -2789,7 +2906,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="34" t="s">
         <v>25</v>
       </c>
@@ -2804,11 +2921,11 @@
       <c r="I17" s="18"/>
       <c r="J17" s="53">
         <f>(C1*((J13+J14+J15)/J13))</f>
-        <v>3.0965330661322645</v>
-      </c>
-      <c r="K17" s="60">
+        <v>1.5074179999999999</v>
+      </c>
+      <c r="K17" s="60" t="e">
         <f ca="1">(C1*((K13+K14+K15)/K13))</f>
-        <v>3.1232681017612522</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L17" s="83" t="s">
         <v>1</v>
@@ -2819,11 +2936,11 @@
       <c r="O17" s="18"/>
       <c r="P17" s="53">
         <f>$C$1*(1+P16/(P14+P15))</f>
-        <v>1.2990680497925309</v>
+        <v>3.5232352941176468</v>
       </c>
       <c r="Q17" s="53">
         <f ca="1">$C$1*(1+Q16/(Q14+Q15))</f>
-        <v>1.3009000000000002</v>
+        <v>3.5231567328918327</v>
       </c>
       <c r="R17" s="92" t="s">
         <v>1</v>
@@ -2844,7 +2961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="34"/>
       <c r="B18" s="19"/>
       <c r="C18" s="18"/>
@@ -2867,7 +2984,7 @@
       <c r="W18" s="18"/>
       <c r="X18" s="17"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="34" t="s">
         <v>6</v>
       </c>
@@ -2875,7 +2992,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="13">
-        <v>5.62</v>
+        <v>4.32</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>58</v>
@@ -2886,7 +3003,7 @@
         <v>17</v>
       </c>
       <c r="I19" s="13">
-        <v>4.99</v>
+        <v>10</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>58</v>
@@ -2897,7 +3014,7 @@
         <v>45</v>
       </c>
       <c r="O19" s="13">
-        <v>2.1</v>
+        <v>4.53</v>
       </c>
       <c r="P19" s="4" t="s">
         <v>58</v>
@@ -2916,7 +3033,7 @@
       <c r="W19" s="18"/>
       <c r="X19" s="17"/>
     </row>
-    <row r="20" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="34" t="s">
         <v>6</v>
       </c>
@@ -2924,7 +3041,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="13">
-        <v>7.32</v>
+        <v>8.8699999999999992</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>58</v>
@@ -2935,7 +3052,7 @@
         <v>18</v>
       </c>
       <c r="I20" s="13">
-        <v>6.65</v>
+        <v>0.78700000000000003</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>58</v>
@@ -2947,7 +3064,7 @@
       </c>
       <c r="O20" s="93">
         <f>O15</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P20" s="4" t="s">
         <v>58</v>
@@ -2967,7 +3084,7 @@
       <c r="W20" s="18"/>
       <c r="X20" s="17"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="34" t="s">
         <v>6</v>
       </c>
@@ -2980,7 +3097,7 @@
         <v>19</v>
       </c>
       <c r="I21" s="13">
-        <v>1.24</v>
+        <v>1.74</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>58</v>
@@ -2991,7 +3108,7 @@
         <v>46</v>
       </c>
       <c r="O21" s="13">
-        <v>0.9</v>
+        <v>8.66</v>
       </c>
       <c r="P21" s="4" t="s">
         <v>58</v>
@@ -3010,7 +3127,7 @@
       <c r="W21" s="18"/>
       <c r="X21" s="17"/>
     </row>
-    <row r="22" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="34"/>
       <c r="B22" s="19"/>
       <c r="C22" s="18"/>
@@ -3040,7 +3157,7 @@
       <c r="W22" s="18"/>
       <c r="X22" s="17"/>
     </row>
-    <row r="23" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="34" t="s">
         <v>51</v>
       </c>
@@ -3049,14 +3166,14 @@
       </c>
       <c r="C23" s="64">
         <f>$C$1*(1+C20/C19)*3/2</f>
-        <v>4.1790213523131667</v>
+        <v>5.5416319444444433</v>
       </c>
       <c r="D23" s="86" t="s">
         <v>1</v>
       </c>
       <c r="E23" s="65">
         <f>(C23-C9)/C23*100</f>
-        <v>-0.50199905476006634</v>
+        <v>0.75125783996138262</v>
       </c>
       <c r="F23" s="84" t="s">
         <v>2</v>
@@ -3066,14 +3183,14 @@
       </c>
       <c r="I23" s="64">
         <f>C1*(1+I20/I19)</f>
-        <v>2.8225250501002006</v>
+        <v>1.3052269999999999</v>
       </c>
       <c r="J23" s="79" t="s">
         <v>1</v>
       </c>
       <c r="K23" s="65">
         <f>(I23-I8)/I23*100</f>
-        <v>0.79804606515010856</v>
+        <v>0.40046673873585747</v>
       </c>
       <c r="L23" s="84" t="s">
         <v>2</v>
@@ -3083,11 +3200,11 @@
       </c>
       <c r="O23" s="64">
         <f>$C$1*(1+O21/(O19+O20))</f>
-        <v>1.2999999999999998</v>
+        <v>3.5231567328918323</v>
       </c>
       <c r="P23" s="65">
         <f>(O23-O9)/O23*100</f>
-        <v>-1.7080354225002411E-14</v>
+        <v>0.65727228867348964</v>
       </c>
       <c r="Q23" s="94" t="s">
         <v>2</v>
@@ -3099,13 +3216,13 @@
       <c r="W23" s="18"/>
       <c r="X23" s="17"/>
     </row>
-    <row r="24" spans="1:28" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
         <v>51</v>
       </c>
       <c r="B24" s="28"/>
-      <c r="C24" s="103"/>
-      <c r="D24" s="103"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
       <c r="E24" s="29"/>
       <c r="F24" s="76"/>
       <c r="H24" s="66" t="s">
@@ -3113,21 +3230,21 @@
       </c>
       <c r="I24" s="77">
         <f>(C1*((I19+I20+I21)/I19))</f>
-        <v>3.1232064128256511</v>
-      </c>
-      <c r="J24" s="105" t="s">
+        <v>1.5157670000000001</v>
+      </c>
+      <c r="J24" s="97" t="s">
         <v>1</v>
       </c>
       <c r="K24" s="78">
         <f>(I24-I9)/I24*100</f>
-        <v>0.74303167188541897</v>
+        <v>1.0401994501793539</v>
       </c>
       <c r="L24" s="82" t="s">
         <v>2</v>
       </c>
       <c r="N24" s="28"/>
-      <c r="O24" s="103"/>
-      <c r="P24" s="103"/>
+      <c r="O24" s="95"/>
+      <c r="P24" s="95"/>
       <c r="Q24" s="29"/>
       <c r="R24" s="76"/>
       <c r="T24" s="66" t="s">
@@ -3148,12 +3265,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="75"/>
       <c r="B25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="22"/>
-      <c r="F25" s="104"/>
+      <c r="F25" s="96"/>
       <c r="G25" s="3"/>
       <c r="I25" s="88"/>
       <c r="J25" s="88"/>
@@ -3169,7 +3286,7 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
     </row>
-    <row r="26" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="20"/>
       <c r="D26" s="21"/>
       <c r="E26" s="35" t="s">
@@ -3184,7 +3301,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B27" s="20"/>
       <c r="D27" s="21"/>
       <c r="E27" s="35" t="s">
@@ -3199,7 +3316,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
       <c r="D28" s="61"/>
@@ -3215,7 +3332,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
       <c r="D29" s="24"/>
@@ -3231,7 +3348,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B30" s="21"/>
       <c r="C30" s="23"/>
       <c r="D30" s="21"/>
@@ -3245,7 +3362,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B31" s="21"/>
       <c r="C31" s="23"/>
       <c r="D31" s="21"/>
@@ -3259,7 +3376,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B32" s="21"/>
       <c r="C32" s="23"/>
       <c r="D32" s="21"/>
@@ -3273,7 +3390,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
       <c r="D33" s="21"/>
@@ -3287,7 +3404,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="34" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B34" s="21"/>
       <c r="C34" s="25"/>
       <c r="D34" s="26"/>
@@ -3301,7 +3418,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B35" s="21"/>
       <c r="C35" s="25"/>
       <c r="D35" s="25"/>
@@ -3315,7 +3432,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:28" x14ac:dyDescent="0.2">
       <c r="AA36" s="5">
         <v>14.7</v>
       </c>
@@ -3323,7 +3440,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="37" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:28" x14ac:dyDescent="0.2">
       <c r="AA37" s="5">
         <v>15</v>
       </c>
@@ -3331,7 +3448,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="38" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:28" x14ac:dyDescent="0.2">
       <c r="AA38" s="5">
         <v>15.4</v>
       </c>
@@ -3339,7 +3456,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:28" x14ac:dyDescent="0.2">
       <c r="AA39" s="5">
         <v>15.8</v>
       </c>
@@ -3347,7 +3464,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="40" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:28" x14ac:dyDescent="0.2">
       <c r="AA40" s="5">
         <v>16.2</v>
       </c>
@@ -3355,7 +3472,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="41" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:28" x14ac:dyDescent="0.2">
       <c r="AA41" s="5">
         <v>16.5</v>
       </c>
@@ -3363,7 +3480,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:28" x14ac:dyDescent="0.2">
       <c r="AA42" s="5">
         <v>16.899999999999999</v>
       </c>
@@ -3371,7 +3488,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="43" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:28" x14ac:dyDescent="0.2">
       <c r="AA43" s="5">
         <v>17.399999999999999</v>
       </c>
@@ -3379,7 +3496,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="44" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:28" x14ac:dyDescent="0.2">
       <c r="AA44" s="5">
         <v>17.8</v>
       </c>
@@ -3387,7 +3504,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="45" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:28" x14ac:dyDescent="0.2">
       <c r="AA45" s="5">
         <v>18.2</v>
       </c>
@@ -3395,7 +3512,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="46" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:28" x14ac:dyDescent="0.2">
       <c r="AA46" s="5">
         <v>18.7</v>
       </c>
@@ -3403,7 +3520,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="47" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:28" x14ac:dyDescent="0.2">
       <c r="AA47" s="5">
         <v>19.100000000000001</v>
       </c>
@@ -3411,7 +3528,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:28" x14ac:dyDescent="0.2">
       <c r="AA48" s="5">
         <v>19.600000000000001</v>
       </c>
@@ -3419,7 +3536,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="49" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA49" s="5">
         <v>20</v>
       </c>
@@ -3427,7 +3544,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="50" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA50" s="5">
         <v>20.5</v>
       </c>
@@ -3435,7 +3552,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="51" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA51" s="5">
         <v>21</v>
       </c>
@@ -3443,7 +3560,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="52" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA52" s="5">
         <v>21.5</v>
       </c>
@@ -3451,7 +3568,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA53" s="5">
         <v>22.1</v>
       </c>
@@ -3459,7 +3576,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="54" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="54" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA54" s="5">
         <v>22.6</v>
       </c>
@@ -3467,7 +3584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA55" s="5">
         <v>23.2</v>
       </c>
@@ -3475,7 +3592,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="56" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA56" s="5">
         <v>23.7</v>
       </c>
@@ -3483,7 +3600,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA57" s="5">
         <v>24.3</v>
       </c>
@@ -3491,7 +3608,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="58" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA58" s="5">
         <v>24.9</v>
       </c>
@@ -3499,7 +3616,7 @@
         <v>22.6</v>
       </c>
     </row>
-    <row r="59" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA59" s="5">
         <v>25.5</v>
       </c>
@@ -3507,7 +3624,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="60" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA60" s="5">
         <v>26.1</v>
       </c>
@@ -3515,7 +3632,7 @@
         <v>23.7</v>
       </c>
     </row>
-    <row r="61" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA61" s="5">
         <v>26.7</v>
       </c>
@@ -3523,7 +3640,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="62" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA62" s="5">
         <v>27.4</v>
       </c>
@@ -3531,7 +3648,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="63" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA63" s="5">
         <v>28</v>
       </c>
@@ -3539,7 +3656,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="64" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA64" s="5">
         <v>28.7</v>
       </c>
@@ -3547,7 +3664,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="65" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="65" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA65" s="5">
         <v>29.4</v>
       </c>
@@ -3555,7 +3672,7 @@
         <v>26.7</v>
       </c>
     </row>
-    <row r="66" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="66" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA66" s="5">
         <v>30.1</v>
       </c>
@@ -3563,7 +3680,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="67" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA67" s="5">
         <v>30.9</v>
       </c>
@@ -3571,7 +3688,7 @@
         <v>27.4</v>
       </c>
     </row>
-    <row r="68" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="68" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA68" s="5">
         <v>31.6</v>
       </c>
@@ -3579,7 +3696,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="69" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA69" s="5">
         <v>32.4</v>
       </c>
@@ -3587,7 +3704,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="70" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="70" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA70" s="5">
         <v>33.200000000000003</v>
       </c>
@@ -3595,7 +3712,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="71" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="71" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA71" s="5">
         <v>34</v>
       </c>
@@ -3603,7 +3720,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="72" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA72" s="5">
         <v>34.799999999999997</v>
       </c>
@@ -3611,7 +3728,7 @@
         <v>30.1</v>
       </c>
     </row>
-    <row r="73" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="73" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA73" s="5">
         <v>35.700000000000003</v>
       </c>
@@ -3619,7 +3736,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="74" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="74" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA74" s="5">
         <v>36.5</v>
       </c>
@@ -3627,7 +3744,7 @@
         <v>31.6</v>
       </c>
     </row>
-    <row r="75" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="75" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA75" s="5">
         <v>37.4</v>
       </c>
@@ -3635,7 +3752,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="76" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="76" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA76" s="5">
         <v>38.299999999999997</v>
       </c>
@@ -3643,7 +3760,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="77" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA77" s="5">
         <v>39.200000000000003</v>
       </c>
@@ -3651,7 +3768,7 @@
         <v>33.200000000000003</v>
       </c>
     </row>
-    <row r="78" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="78" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA78" s="5">
         <v>40.200000000000003</v>
       </c>
@@ -3659,7 +3776,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="79" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA79" s="5">
         <v>41.2</v>
       </c>
@@ -3667,7 +3784,7 @@
         <v>34.799999999999997</v>
       </c>
     </row>
-    <row r="80" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="80" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA80" s="5">
         <v>42.2</v>
       </c>
@@ -3675,7 +3792,7 @@
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="81" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="81" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA81" s="5">
         <v>43.2</v>
       </c>
@@ -3683,7 +3800,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="82" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="82" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA82" s="5">
         <v>44.2</v>
       </c>
@@ -3691,7 +3808,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="83" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="83" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA83" s="5">
         <v>45.3</v>
       </c>
@@ -3699,7 +3816,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="84" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="84" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA84" s="5">
         <v>46.4</v>
       </c>
@@ -3707,7 +3824,7 @@
         <v>38.299999999999997</v>
       </c>
     </row>
-    <row r="85" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="85" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA85" s="5">
         <v>47.5</v>
       </c>
@@ -3715,7 +3832,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="86" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="86" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA86" s="5">
         <v>48.7</v>
       </c>
@@ -3723,7 +3840,7 @@
         <v>39.200000000000003</v>
       </c>
     </row>
-    <row r="87" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="87" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA87" s="5">
         <v>49.9</v>
       </c>
@@ -3731,7 +3848,7 @@
         <v>40.200000000000003</v>
       </c>
     </row>
-    <row r="88" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="88" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA88" s="5">
         <v>51.1</v>
       </c>
@@ -3739,7 +3856,7 @@
         <v>41.2</v>
       </c>
     </row>
-    <row r="89" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="89" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA89" s="5">
         <v>52.3</v>
       </c>
@@ -3747,7 +3864,7 @@
         <v>42.2</v>
       </c>
     </row>
-    <row r="90" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="90" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA90" s="5">
         <v>53.6</v>
       </c>
@@ -3755,7 +3872,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="91" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="91" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA91" s="5">
         <v>54.9</v>
       </c>
@@ -3763,7 +3880,7 @@
         <v>43.2</v>
       </c>
     </row>
-    <row r="92" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="92" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA92" s="5">
         <v>56.2</v>
       </c>
@@ -3771,7 +3888,7 @@
         <v>44.2</v>
       </c>
     </row>
-    <row r="93" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="93" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA93" s="5">
         <v>57.6</v>
       </c>
@@ -3779,7 +3896,7 @@
         <v>45.3</v>
       </c>
     </row>
-    <row r="94" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="94" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA94" s="5">
         <v>59</v>
       </c>
@@ -3787,7 +3904,7 @@
         <v>46.4</v>
       </c>
     </row>
-    <row r="95" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="95" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA95" s="5">
         <v>60.4</v>
       </c>
@@ -3795,7 +3912,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="96" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="96" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA96" s="5">
         <v>61.9</v>
       </c>
@@ -3803,7 +3920,7 @@
         <v>47.5</v>
       </c>
     </row>
-    <row r="97" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="97" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA97" s="5">
         <v>63.4</v>
       </c>
@@ -3811,7 +3928,7 @@
         <v>48.7</v>
       </c>
     </row>
-    <row r="98" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="98" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA98" s="5">
         <v>64.900000000000006</v>
       </c>
@@ -3819,7 +3936,7 @@
         <v>49.9</v>
       </c>
     </row>
-    <row r="99" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="99" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA99" s="5">
         <v>66.5</v>
       </c>
@@ -3827,7 +3944,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="100" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="100" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA100" s="5">
         <v>68.099999999999994</v>
       </c>
@@ -3835,7 +3952,7 @@
         <v>51.1</v>
       </c>
     </row>
-    <row r="101" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="101" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA101" s="5">
         <v>69.8</v>
       </c>
@@ -3843,7 +3960,7 @@
         <v>52.3</v>
       </c>
     </row>
-    <row r="102" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="102" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA102" s="5">
         <v>71.5</v>
       </c>
@@ -3851,7 +3968,7 @@
         <v>53.6</v>
       </c>
     </row>
-    <row r="103" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="103" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA103" s="5">
         <v>73.2</v>
       </c>
@@ -3859,7 +3976,7 @@
         <v>54.9</v>
       </c>
     </row>
-    <row r="104" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="104" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA104" s="5">
         <v>75</v>
       </c>
@@ -3867,7 +3984,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="105" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="105" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA105" s="5">
         <v>76.8</v>
       </c>
@@ -3875,7 +3992,7 @@
         <v>56.2</v>
       </c>
     </row>
-    <row r="106" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="106" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA106" s="5">
         <v>78.7</v>
       </c>
@@ -3883,7 +4000,7 @@
         <v>57.6</v>
       </c>
     </row>
-    <row r="107" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="107" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA107" s="5">
         <v>80.599999999999994</v>
       </c>
@@ -3891,7 +4008,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="108" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="108" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA108" s="5">
         <v>82.5</v>
       </c>
@@ -3899,7 +4016,7 @@
         <v>60.4</v>
       </c>
     </row>
-    <row r="109" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="109" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA109" s="5">
         <v>84.5</v>
       </c>
@@ -3907,7 +4024,7 @@
         <v>61.9</v>
       </c>
     </row>
-    <row r="110" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="110" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA110" s="5">
         <v>86.6</v>
       </c>
@@ -3915,7 +4032,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="111" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="111" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA111" s="5">
         <v>88.7</v>
       </c>
@@ -3923,7 +4040,7 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="112" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="112" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA112" s="5">
         <v>90.9</v>
       </c>
@@ -3931,7 +4048,7 @@
         <v>64.900000000000006</v>
       </c>
     </row>
-    <row r="113" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="113" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA113" s="5">
         <v>93.1</v>
       </c>
@@ -3939,7 +4056,7 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="114" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="114" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA114" s="5">
         <v>95.3</v>
       </c>
@@ -3947,7 +4064,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="115" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="115" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA115" s="5">
         <v>97.6</v>
       </c>
@@ -3955,7 +4072,7 @@
         <v>68.099999999999994</v>
       </c>
     </row>
-    <row r="116" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="116" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA116" s="5">
         <v>100</v>
       </c>
@@ -3963,126 +4080,126 @@
         <v>69.8</v>
       </c>
     </row>
-    <row r="117" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="117" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA117" s="5"/>
       <c r="AB117" s="5">
         <v>71.5</v>
       </c>
     </row>
-    <row r="118" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="118" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA118" s="5"/>
       <c r="AB118" s="5">
         <v>73.2</v>
       </c>
     </row>
-    <row r="119" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="119" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA119" s="5"/>
       <c r="AB119" s="5">
         <v>75</v>
       </c>
     </row>
-    <row r="120" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="120" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA120" s="5"/>
       <c r="AB120" s="5">
         <v>76.8</v>
       </c>
     </row>
-    <row r="121" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="121" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA121" s="5"/>
       <c r="AB121" s="5">
         <v>78.7</v>
       </c>
     </row>
-    <row r="122" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="122" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA122" s="5"/>
       <c r="AB122" s="5">
         <v>80.599999999999994</v>
       </c>
     </row>
-    <row r="123" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="123" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA123" s="5"/>
       <c r="AB123" s="5">
         <v>82</v>
       </c>
     </row>
-    <row r="124" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="124" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA124" s="5"/>
       <c r="AB124" s="5">
         <v>82.5</v>
       </c>
     </row>
-    <row r="125" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="125" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA125" s="5"/>
       <c r="AB125" s="5">
         <v>84.5</v>
       </c>
     </row>
-    <row r="126" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="126" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA126" s="5"/>
       <c r="AB126" s="5">
         <v>86.6</v>
       </c>
     </row>
-    <row r="127" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="127" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA127" s="5"/>
       <c r="AB127" s="5">
         <v>88.7</v>
       </c>
     </row>
-    <row r="128" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="128" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA128" s="5"/>
       <c r="AB128" s="5">
         <v>90.9</v>
       </c>
     </row>
-    <row r="129" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="129" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA129" s="5"/>
       <c r="AB129" s="5">
         <v>91</v>
       </c>
     </row>
-    <row r="130" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="130" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA130" s="5"/>
       <c r="AB130" s="5">
         <v>93.1</v>
       </c>
     </row>
-    <row r="131" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="131" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA131" s="5"/>
       <c r="AB131" s="5">
         <v>95.3</v>
       </c>
     </row>
-    <row r="132" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="132" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AA132" s="5"/>
       <c r="AB132" s="5">
         <v>97.6</v>
       </c>
     </row>
-    <row r="133" spans="27:28" x14ac:dyDescent="0.25">
+    <row r="133" spans="27:28" x14ac:dyDescent="0.2">
       <c r="AB133" s="27">
         <v>100</v>
       </c>
     </row>
-    <row r="147" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H147" s="2"/>
     </row>
-    <row r="148" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H148" s="2"/>
     </row>
-    <row r="149" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H149" s="2"/>
     </row>
-    <row r="150" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H150" s="2"/>
     </row>
-    <row r="151" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H151" s="2"/>
     </row>
-    <row r="152" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H152" s="2"/>
     </row>
-    <row r="153" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H153" s="2"/>
     </row>
   </sheetData>
@@ -4111,13 +4228,13 @@
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>114300</xdr:colOff>
                 <xdr:row>30</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:rowOff>101600</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>22</xdr:col>
-                <xdr:colOff>104775</xdr:colOff>
+                <xdr:colOff>101600</xdr:colOff>
                 <xdr:row>65</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
+                <xdr:rowOff>165100</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -4132,14 +4249,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J32" sqref="J29:J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Schematic finished, components added, PCB design started
</commit_message>
<xml_diff>
--- a/bq25505(70_Design_Help_V1_3.xlsx
+++ b/bq25505(70_Design_Help_V1_3.xlsx
@@ -1327,7 +1327,7 @@
         <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1380,7 +1380,7 @@
         <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1433,7 +1433,7 @@
         <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1486,7 +1486,7 @@
         <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1539,7 +1539,7 @@
         <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1592,7 +1592,7 @@
         <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1645,7 +1645,7 @@
         <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000012000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1698,7 +1698,7 @@
         <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1751,7 +1751,7 @@
         <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000011000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1804,7 +1804,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1862,7 +1862,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2188,7 +2188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I19" sqref="I19"/>
+      <selection pane="topRight" activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2979,7 +2979,7 @@
         <v>45</v>
       </c>
       <c r="O19" s="13">
-        <v>4.53</v>
+        <v>4.42</v>
       </c>
       <c r="P19" s="4" t="s">
         <v>58</v>
@@ -3073,7 +3073,7 @@
         <v>46</v>
       </c>
       <c r="O21" s="13">
-        <v>8.66</v>
+        <v>8.4499999999999993</v>
       </c>
       <c r="P21" s="4" t="s">
         <v>58</v>
@@ -3165,11 +3165,11 @@
       </c>
       <c r="O23" s="64">
         <f>$C$1*(1+O21/(O19+O20))</f>
-        <v>3.5231567328918323</v>
+        <v>3.5232352941176468</v>
       </c>
       <c r="P23" s="65">
         <f>(O23-O9)/O23*100</f>
-        <v>0.65727228867348964</v>
+        <v>0.65948743634693319</v>
       </c>
       <c r="Q23" s="94" t="s">
         <v>2</v>

</xml_diff>